<commit_message>
Added udp sender run 1 to 5
</commit_message>
<xml_diff>
--- a/BA1 Refactoring Experiment Ergebnisse/ExcelAuswertung.xlsx
+++ b/BA1 Refactoring Experiment Ergebnisse/ExcelAuswertung.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onura\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onura\source\repos\BA1-Results\BA1 Refactoring Experiment Ergebnisse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6748BF-F533-4FD8-886F-9BAF3D578DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A96D689-8ACF-48BD-855A-5729917B0EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9840" yWindow="2715" windowWidth="34020" windowHeight="15345" activeTab="1" xr2:uid="{02DB93EE-99D6-4721-B868-1DDC079EB0CD}"/>
+    <workbookView xWindow="2145" yWindow="3105" windowWidth="34020" windowHeight="15345" activeTab="1" xr2:uid="{02DB93EE-99D6-4721-B868-1DDC079EB0CD}"/>
   </bookViews>
   <sheets>
     <sheet name="JSON Reader Code Beispiel" sheetId="1" r:id="rId1"/>
-    <sheet name="2.Beispiel" sheetId="2" r:id="rId2"/>
+    <sheet name="UDP Sender Code Beispiel" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -491,7 +491,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="A1:D35"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,7 +960,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,6 +983,12 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>60</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
       <c r="D2" t="str">
         <f>IF(C2:C26&gt;0,"Yes","No")</f>
         <v>No</v>
@@ -992,6 +998,12 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>59</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D26" si="0">IF(C3:C28&gt;0,"Yes","No")</f>
         <v>No</v>
@@ -1001,6 +1013,12 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>60</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -1010,15 +1028,27 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
+      <c r="B5">
+        <v>65</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
+      <c r="B6">
+        <v>63</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -1208,13 +1238,13 @@
       <c r="A28" t="s">
         <v>28</v>
       </c>
-      <c r="B28" t="e">
+      <c r="B28">
         <f>AVERAGE(B2:B26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C28" t="e">
+        <v>61.4</v>
+      </c>
+      <c r="C28">
         <f>AVERAGE(C2:C26)</f>
-        <v>#DIV/0!</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1223,7 +1253,7 @@
       </c>
       <c r="B29">
         <f>MIN(B2:B26)</f>
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="C29">
         <f>MIN(C2:C26)</f>
@@ -1236,11 +1266,11 @@
       </c>
       <c r="B30">
         <f>MAX(B2:B26)</f>
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="C30">
         <f>MAX(C2:C26)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1257,9 +1287,9 @@
       <c r="A35" t="s">
         <v>34</v>
       </c>
-      <c r="B35" t="e">
+      <c r="B35">
         <f>_xlfn.STDEV.P(B2:B26)</f>
-        <v>#DIV/0!</v>
+        <v>2.2449944320643649</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished UDP Sender example
</commit_message>
<xml_diff>
--- a/BA1 Refactoring Experiment Ergebnisse/ExcelAuswertung.xlsx
+++ b/BA1 Refactoring Experiment Ergebnisse/ExcelAuswertung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onura\source\repos\BA1-Results\BA1 Refactoring Experiment Ergebnisse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A96D689-8ACF-48BD-855A-5729917B0EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4A00CD-E5AE-4A77-BDA3-F41493E3387D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="3105" windowWidth="34020" windowHeight="15345" activeTab="1" xr2:uid="{02DB93EE-99D6-4721-B868-1DDC079EB0CD}"/>
+    <workbookView xWindow="2760" yWindow="1575" windowWidth="34020" windowHeight="15345" activeTab="1" xr2:uid="{02DB93EE-99D6-4721-B868-1DDC079EB0CD}"/>
   </bookViews>
   <sheets>
     <sheet name="JSON Reader Code Beispiel" sheetId="1" r:id="rId1"/>
@@ -491,7 +491,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,6 +929,7 @@
         <v>32</v>
       </c>
       <c r="B32">
+        <f>COUNTIF(D2:D26,"Yes")</f>
         <v>10</v>
       </c>
     </row>
@@ -937,6 +938,7 @@
         <v>33</v>
       </c>
       <c r="B33">
+        <f>COUNTIF(D2:D26,"No")</f>
         <v>15</v>
       </c>
     </row>
@@ -960,7 +962,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1058,6 +1060,12 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="B7">
+        <v>61</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -1067,6 +1075,12 @@
       <c r="A8" t="s">
         <v>7</v>
       </c>
+      <c r="B8">
+        <v>63</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -1076,6 +1090,12 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
+      <c r="B9">
+        <v>69</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -1085,6 +1105,12 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
+      <c r="B10">
+        <v>56</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -1094,6 +1120,12 @@
       <c r="A11" t="s">
         <v>10</v>
       </c>
+      <c r="B11">
+        <v>61</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -1103,15 +1135,27 @@
       <c r="A12" t="s">
         <v>11</v>
       </c>
+      <c r="B12">
+        <v>58</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
+      <c r="B13">
+        <v>55</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -1121,6 +1165,12 @@
       <c r="A14" t="s">
         <v>13</v>
       </c>
+      <c r="B14">
+        <v>65</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -1130,6 +1180,12 @@
       <c r="A15" t="s">
         <v>14</v>
       </c>
+      <c r="B15">
+        <v>60</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -1139,6 +1195,12 @@
       <c r="A16" t="s">
         <v>15</v>
       </c>
+      <c r="B16">
+        <v>67</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -1148,6 +1210,12 @@
       <c r="A17" t="s">
         <v>16</v>
       </c>
+      <c r="B17">
+        <v>56</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -1157,6 +1225,12 @@
       <c r="A18" t="s">
         <v>17</v>
       </c>
+      <c r="B18">
+        <v>65</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -1166,6 +1240,12 @@
       <c r="A19" t="s">
         <v>18</v>
       </c>
+      <c r="B19">
+        <v>65</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -1175,6 +1255,12 @@
       <c r="A20" t="s">
         <v>19</v>
       </c>
+      <c r="B20">
+        <v>75</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -1184,6 +1270,12 @@
       <c r="A21" t="s">
         <v>20</v>
       </c>
+      <c r="B21">
+        <v>66</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -1193,6 +1285,12 @@
       <c r="A22" t="s">
         <v>21</v>
       </c>
+      <c r="B22">
+        <v>60</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -1202,6 +1300,12 @@
       <c r="A23" t="s">
         <v>22</v>
       </c>
+      <c r="B23">
+        <v>56</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -1211,6 +1315,12 @@
       <c r="A24" t="s">
         <v>23</v>
       </c>
+      <c r="B24">
+        <v>63</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -1220,15 +1330,27 @@
       <c r="A25" t="s">
         <v>24</v>
       </c>
+      <c r="B25">
+        <v>65</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
+      <c r="B26">
+        <v>56</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -1240,11 +1362,11 @@
       </c>
       <c r="B28">
         <f>AVERAGE(B2:B26)</f>
-        <v>61.4</v>
+        <v>61.96</v>
       </c>
       <c r="C28">
         <f>AVERAGE(C2:C26)</f>
-        <v>1.2</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1253,7 +1375,7 @@
       </c>
       <c r="B29">
         <f>MIN(B2:B26)</f>
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C29">
         <f>MIN(C2:C26)</f>
@@ -1266,7 +1388,7 @@
       </c>
       <c r="B30">
         <f>MAX(B2:B26)</f>
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C30">
         <f>MAX(C2:C26)</f>
@@ -1277,11 +1399,19 @@
       <c r="A32" t="s">
         <v>32</v>
       </c>
+      <c r="B32">
+        <f>COUNTIF(D2:D26,"Yes")</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
+      <c r="B33">
+        <f>COUNTIF(D2:D26,"No")</f>
+        <v>22</v>
+      </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -1289,7 +1419,7 @@
       </c>
       <c r="B35">
         <f>_xlfn.STDEV.P(B2:B26)</f>
-        <v>2.2449944320643649</v>
+        <v>4.6603004195008726</v>
       </c>
     </row>
   </sheetData>

</xml_diff>